<commit_message>
Update to v 6.2
</commit_message>
<xml_diff>
--- a/EnviroHATv6/EnviroHatv6_bom.xlsx
+++ b/EnviroHATv6/EnviroHatv6_bom.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="82">
   <si>
     <t xml:space="preserve">Comment</t>
   </si>
@@ -115,7 +115,7 @@
     <t xml:space="preserve">C2297 </t>
   </si>
   <si>
-    <t xml:space="preserve">R4,R17,R15,R10,R21,R5,R3,R16,R24,R26</t>
+    <t xml:space="preserve">R4,R17,R15,R10,R21,R5,R3,R16,R24,R26,R28,R29</t>
   </si>
   <si>
     <t xml:space="preserve">R_1206_3216Metric_Pad1.30x1.75mm_HandSolder</t>
@@ -184,16 +184,19 @@
     <t xml:space="preserve">3k6</t>
   </si>
   <si>
-    <t xml:space="preserve">R2,R1</t>
+    <t xml:space="preserve">R2,R1,R9,R27</t>
   </si>
   <si>
     <t xml:space="preserve">C176265 </t>
   </si>
   <si>
+    <t xml:space="preserve">1k</t>
+  </si>
+  <si>
     <t xml:space="preserve">R11</t>
   </si>
   <si>
-    <t xml:space="preserve">C17909 </t>
+    <t xml:space="preserve">C4410</t>
   </si>
   <si>
     <t xml:space="preserve">XC6206P332MR</t>
@@ -414,32 +417,36 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -523,337 +530,337 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8828125" defaultRowHeight="20" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="24.47"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="72.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="36.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="24.47"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+    <row r="2" s="7" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" s="7" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" s="7" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="C4" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+    <row r="5" s="7" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+    <row r="6" s="7" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="C6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+    <row r="7" s="7" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" s="6" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="n">
+    <row r="8" s="7" customFormat="true" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="2" t="n">
         <v>470</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="C9" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="C10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="C11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="C12" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>120</v>
-      </c>
-      <c r="B13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="0" t="s">
+      <c r="B13" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>44</v>
+      <c r="D13" s="6" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="A14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="0" t="s">
+      <c r="B14" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="D14" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B15" s="0" t="s">
+      <c r="A15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="0" t="s">
+      <c r="B15" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="5" t="s">
-        <v>51</v>
+      <c r="D15" s="6" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16" s="0" t="s">
+      <c r="A16" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="0" t="s">
+      <c r="B16" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="C16" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="D16" s="6" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="0" t="s">
+      <c r="A17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="D17" s="0" t="s">
+      <c r="B17" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="0" t="s">
+      <c r="A18" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="0" t="s">
+      <c r="B18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="C18" s="2" t="s">
         <v>62</v>
       </c>
+      <c r="D18" s="6" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B19" s="0" t="s">
+      <c r="A19" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="B19" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="C19" s="2" t="s">
         <v>66</v>
       </c>
+      <c r="D19" s="6" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B20" s="0" t="s">
+      <c r="A20" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="B20" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D20" s="5" t="s">
-        <v>69</v>
+      <c r="D20" s="6" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="0" t="s">
+      <c r="A21" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="B21" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="C21" s="2" t="s">
         <v>73</v>
       </c>
+      <c r="D21" s="6" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="B22" s="4" t="s">
+      <c r="A22" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="B22" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>76</v>
+      <c r="D22" s="6" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="20" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="s">
-        <v>77</v>
-      </c>
-      <c r="B23" s="0" t="s">
+      <c r="A23" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="B23" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="C23" s="2" t="s">
         <v>80</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>

</xml_diff>